<commit_message>
Add Sub Groups Initial Build
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" activeTab="7"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="210">
   <si>
     <t>Key</t>
   </si>
@@ -3394,7 +3394,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3427,9 +3427,6 @@
       </c>
       <c r="B3" t="s">
         <v>189</v>
-      </c>
-      <c r="C3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3544,7 +3541,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created workflow for TS_AL_04, Create List_Contacts
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" tabRatio="739" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" tabRatio="923" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,9 @@
     <sheet name="Filters" sheetId="12" r:id="rId7"/>
     <sheet name="Groups Data" sheetId="13" r:id="rId8"/>
     <sheet name="Group List Data" sheetId="14" r:id="rId9"/>
-    <sheet name="List Data" sheetId="7" r:id="rId10"/>
-    <sheet name="Prospect Data" sheetId="4" r:id="rId11"/>
+    <sheet name="Group List Data- Contacts" sheetId="15" r:id="rId10"/>
+    <sheet name="List Data" sheetId="7" r:id="rId11"/>
+    <sheet name="Prospect Data" sheetId="4" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="Budget_Revenue">Filters!$F$2:$F$9</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="225">
   <si>
     <t>Key</t>
   </si>
@@ -558,9 +559,6 @@
     <t>Is less than</t>
   </si>
   <si>
-    <t>Is null</t>
-  </si>
-  <si>
     <t>Is not null</t>
   </si>
   <si>
@@ -627,21 +625,12 @@
     <t>https://lamb-uat.azurewebsites.net/</t>
   </si>
   <si>
-    <t>Groups</t>
-  </si>
-  <si>
     <t>All filtered prospect must Satisfy Conditions of Defined Groups</t>
   </si>
   <si>
-    <t>New Dynamic List-NJ-Over-1000002</t>
-  </si>
-  <si>
     <t>Group3</t>
   </si>
   <si>
-    <t>Group1,Group2,Group3</t>
-  </si>
-  <si>
     <t>Group2,Group3</t>
   </si>
   <si>
@@ -717,7 +706,79 @@
     <t>N</t>
   </si>
   <si>
-    <t>Group1,Group2</t>
+    <t>Group1,Group2,Group3,Group4</t>
+  </si>
+  <si>
+    <t>New Dynamic List-NJ-Over-1000017</t>
+  </si>
+  <si>
+    <t>New Dynamic List-NJ-Over-1000018</t>
+  </si>
+  <si>
+    <t>Group2,Group3,Group4</t>
+  </si>
+  <si>
+    <t>Filter#</t>
+  </si>
+  <si>
+    <t>Filter1</t>
+  </si>
+  <si>
+    <t>Filter2</t>
+  </si>
+  <si>
+    <t>Filter3</t>
+  </si>
+  <si>
+    <t>Filter4</t>
+  </si>
+  <si>
+    <t>Filter5</t>
+  </si>
+  <si>
+    <t>Filter6</t>
+  </si>
+  <si>
+    <t>Filter7</t>
+  </si>
+  <si>
+    <t>Groups and Filters</t>
+  </si>
+  <si>
+    <t>TS_AL_04</t>
+  </si>
+  <si>
+    <t>All filtered contacts must Satisfy Conditions of Defined Groups</t>
+  </si>
+  <si>
+    <t>Validate that users added during the "Add List" wizard are correctly assigned the contact.</t>
+  </si>
+  <si>
+    <t>User are correctly assigned contacts.</t>
+  </si>
+  <si>
+    <t>Group2,Group4</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Group5,Group1,Group2</t>
+  </si>
+  <si>
+    <t>Group1,group3</t>
+  </si>
+  <si>
+    <t>New Dynamic List-NJ-Over-1000036</t>
+  </si>
+  <si>
+    <t>New Dynamic List-NJ-Over-1000037</t>
+  </si>
+  <si>
+    <t>Kevin Corona,Manoj Peruri</t>
+  </si>
+  <si>
+    <t>New Dynamic List-NJ-Over-1000042</t>
   </si>
 </sst>
 </file>
@@ -782,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -826,6 +887,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1116,7 +1183,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1192,7 @@
     <col min="2" max="2" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1141,9 +1208,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>76</v>
@@ -1157,10 +1224,154 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="6" width="31.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>"And,Or"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1388,7 @@
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>51</v>
       </c>
@@ -1209,7 +1420,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1237,7 +1448,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1265,7 +1476,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
@@ -1298,7 +1509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1314,7 +1525,7 @@
     <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>92</v>
       </c>
@@ -1334,9 +1545,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>97</v>
@@ -1354,52 +1565,52 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F3" s="1">
         <v>3250000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F4" s="1">
         <v>4250000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>98</v>
@@ -1414,12 +1625,12 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>98</v>
@@ -1444,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1665,7 @@
     <col min="2" max="16384" width="34.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1494,7 +1705,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>16</v>
@@ -1520,7 +1731,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>23</v>
@@ -1549,9 +1760,9 @@
         <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1578,9 +1789,9 @@
         <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="18"/>
+        <v>199</v>
+      </c>
+      <c r="C5" s="20"/>
       <c r="D5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1592,23 +1803,23 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="345" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18" t="s">
+      <c r="B6" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="20" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="20" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -1619,15 +1830,15 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="3" t="s">
         <v>45</v>
       </c>
@@ -1636,15 +1847,15 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="18"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="3" t="s">
         <v>47</v>
       </c>
@@ -1653,15 +1864,15 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1670,13 +1881,21 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="18" t="s">
+        <v>215</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="18" t="s">
+        <v>216</v>
+      </c>
       <c r="J10" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1685,11 +1904,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G6:G9"/>
-    <mergeCell ref="C4:C9"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C4:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1712,7 +1931,7 @@
     <col min="7" max="7" width="29.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1744,7 +1963,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1771,7 +1990,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -1799,7 +2018,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
@@ -1827,7 +2046,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H6" s="9"/>
     </row>
   </sheetData>
@@ -1849,7 +2068,7 @@
     <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -1857,7 +2076,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
@@ -1865,7 +2084,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>62</v>
       </c>
@@ -1873,7 +2092,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>70</v>
       </c>
@@ -1881,7 +2100,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>58</v>
       </c>
@@ -1889,7 +2108,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>72</v>
       </c>
@@ -1897,7 +2116,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>73</v>
       </c>
@@ -1905,12 +2124,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1933,7 +2152,7 @@
     <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -1941,7 +2160,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -1949,12 +2168,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1988,7 +2207,7 @@
     <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>51</v>
       </c>
@@ -2020,7 +2239,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -2048,7 +2267,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -2076,7 +2295,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
@@ -2114,16 +2333,16 @@
   <dimension ref="A1:AK14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="33" style="15" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="15"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33" style="15" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="15"/>
     <col min="6" max="6" width="13.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" hidden="1" customWidth="1"/>
     <col min="8" max="13" width="0" hidden="1" customWidth="1"/>
@@ -2133,17 +2352,20 @@
     <col min="18" max="37" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
@@ -2180,7 +2402,7 @@
         <v>126</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>127</v>
@@ -2243,18 +2465,21 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>153</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>168</v>
+        <v>152</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>167</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>145</v>
@@ -2275,7 +2500,7 @@
         <v>145</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>145</v>
@@ -2287,7 +2512,7 @@
         <v>145</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>145</v>
@@ -2353,15 +2578,18 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>160</v>
+      <c r="D3" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>146</v>
@@ -2382,7 +2610,7 @@
         <v>146</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M3" s="13" t="s">
         <v>146</v>
@@ -2394,7 +2622,7 @@
         <v>146</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q3" s="13" t="s">
         <v>146</v>
@@ -2460,30 +2688,33 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>154</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>167</v>
+        <v>153</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>147</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>147</v>
@@ -2492,108 +2723,111 @@
         <v>147</v>
       </c>
       <c r="L4" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="M4" s="13" t="s">
-        <v>162</v>
-      </c>
       <c r="N4" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R4" s="13" t="s">
         <v>147</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U4" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AB4" s="13" t="s">
         <v>147</v>
       </c>
       <c r="AC4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AD4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AG4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AH4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AI4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AJ4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AK4" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="15">
+      <c r="E5" s="15">
         <v>50</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>148</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>148</v>
@@ -2603,103 +2837,106 @@
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R5" s="13" t="s">
         <v>148</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB5" s="13" t="s">
         <v>148</v>
       </c>
       <c r="AC5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AH5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AJ5" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AK5" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="15">
+      <c r="E6" s="15">
         <v>0.5</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>149</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>149</v>
@@ -2709,100 +2946,106 @@
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P6" s="13"/>
       <c r="Q6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R6" s="13" t="s">
         <v>149</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U6" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="W6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AB6" s="13" t="s">
         <v>149</v>
       </c>
       <c r="AC6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AD6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AE6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AF6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AH6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AI6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AJ6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AK6" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>138</v>
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>210</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>153</v>
+        <v>142</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>167</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>150</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>150</v>
@@ -2812,277 +3055,247 @@
       </c>
       <c r="L7" s="13"/>
       <c r="M7" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R7" s="13" t="s">
         <v>150</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U7" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Y7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AB7" s="13" t="s">
         <v>150</v>
       </c>
       <c r="AC7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AG7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AH7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AI7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AJ7" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AK7" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="F8" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="19">
+        <v>200000</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K9" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="T8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="U8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="V8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="W8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="X8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AD8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AG8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AH8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ8" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK8" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="F9" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>152</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P9" s="13"/>
       <c r="Q9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="V9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="W9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AA9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AB9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AC9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AD9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AE9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AF9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AH9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AI9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AJ9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AK9" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -3092,71 +3305,71 @@
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R10" s="13"/>
       <c r="S10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AB10" s="13"/>
       <c r="AC10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AD10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AF10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AI10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AJ10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AK10" s="13"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -3166,62 +3379,62 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R11" s="13"/>
       <c r="S11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U11" s="13"/>
       <c r="V11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="X11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AA11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AD11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AE11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AF11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AG11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AH11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AI11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AJ11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AK11" s="13"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -3255,7 +3468,7 @@
       <c r="AJ12" s="13"/>
       <c r="AK12" s="13"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -3289,7 +3502,7 @@
       <c r="AJ13" s="13"/>
       <c r="AK13" s="13"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -3327,14 +3540,14 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>$F$1:$AK$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C926:C1048576">
-      <formula1>INDIRECT($B:$B)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D926:D1048576">
+      <formula1>INDIRECT($C:$C)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C925">
-      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B2,"?","")," ","_"),"/","_"),"-","_"),".",""))</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D925">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C2,"?","")," ","_"),"/","_"),"-","_"),".",""))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>Group</formula1>
@@ -3350,7 +3563,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3358,7 +3571,7 @@
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>115</v>
       </c>
@@ -3366,113 +3579,113 @@
         <v>54</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>180</v>
       </c>
-      <c r="B5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>169</v>
       </c>
-      <c r="C6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
       <c r="C8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" t="s">
         <v>181</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" t="s">
         <v>169</v>
-      </c>
-      <c r="C11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" t="s">
-        <v>170</v>
       </c>
       <c r="C12" t="s">
         <v>117</v>
@@ -3494,22 +3707,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="4" max="5" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>51</v>
       </c>
@@ -3520,88 +3733,105 @@
         <v>54</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="I2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"And,Or"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Exception Handling and Moved Config to the desktop of current user
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" tabRatio="923" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" tabRatio="923"/>
   </bookViews>
   <sheets>
-    <sheet name="Config" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="Test Scenarios" sheetId="10" r:id="rId2"/>
     <sheet name="Test User Level Data" sheetId="6" state="hidden" r:id="rId3"/>
     <sheet name="Credentials" sheetId="5" r:id="rId4"/>
     <sheet name="URL" sheetId="2" r:id="rId5"/>
     <sheet name="Action Data" sheetId="9" state="hidden" r:id="rId6"/>
-    <sheet name="Groups Data" sheetId="13" r:id="rId7"/>
-    <sheet name="Group List Data- Contacts" sheetId="15" state="hidden" r:id="rId8"/>
-    <sheet name="Group List Data" sheetId="14" r:id="rId9"/>
+    <sheet name="Group List Data- Contacts" sheetId="15" state="hidden" r:id="rId7"/>
+    <sheet name="Group List Data" sheetId="14" r:id="rId8"/>
+    <sheet name="Groups Data" sheetId="13" r:id="rId9"/>
     <sheet name="Filters" sheetId="12" r:id="rId10"/>
     <sheet name="List Data" sheetId="7" state="hidden" r:id="rId11"/>
     <sheet name="Prospect Data" sheetId="4" r:id="rId12"/>
@@ -748,12 +748,6 @@
     <t>Contacts</t>
   </si>
   <si>
-    <t xml:space="preserve">Whiteboard List - Mod  0.5 </t>
-  </si>
-  <si>
-    <t>Contact List - Rev 200K</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -767,6 +761,12 @@
   </si>
   <si>
     <t>Group List Data</t>
+  </si>
+  <si>
+    <t>Contact List - Rev LT 200K</t>
+  </si>
+  <si>
+    <t>Whiteboard List - Mod  0.6</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,6 +1224,9 @@
         <v>74</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1235,7 +1238,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,13 +1331,13 @@
         <v>197</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E5" s="15">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,7 +1368,7 @@
         <v>116</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E7" s="19">
         <v>200000</v>
@@ -1705,7 +1708,7 @@
         <v>90</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>117</v>
@@ -2370,96 +2373,96 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="R8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="U8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="V8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="W8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="X8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Y8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Z8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AA8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AB8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AC8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AD8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AF8" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -2633,13 +2636,13 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -2649,58 +2652,58 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="S11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="V11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="W11" s="13"/>
       <c r="X11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Y11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Z11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AA11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AB11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AC11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AD11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AE11" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AF11" s="13"/>
     </row>
@@ -2781,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2925,10 +2928,10 @@
         <v>40</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>21</v>
@@ -3463,153 +3466,6 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="15.42578125" style="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>"And,Or"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
-      <formula1>Group</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3734,12 +3590,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3792,7 +3648,7 @@
         <v>211</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>209</v>
@@ -3823,7 +3679,7 @@
         <v>212</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>213</v>
@@ -3864,4 +3720,151 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.42578125" style="21" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+      <formula1>"And,Or"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>Group</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>